<commit_message>
included IBP Level 7
</commit_message>
<xml_diff>
--- a/map.xlsx
+++ b/map.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stryker-my.sharepoint.com/personal/swastik_mishra_stryker_com/Documents/python/autoinsights/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="58" documentId="13_ncr:1_{FEDAD199-E267-4A23-A1C7-5876348D1EB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A97A6A08-95BD-4D81-8143-64FC51024E42}"/>
+  <xr:revisionPtr revIDLastSave="76" documentId="13_ncr:1_{FEDAD199-E267-4A23-A1C7-5876348D1EB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D0C30C8F-6888-4BE0-9356-D727DCBB1F7A}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="59">
   <si>
     <t>Location Hierarchy</t>
   </si>
@@ -206,6 +206,15 @@
   </si>
   <si>
     <t>SONICFUSION</t>
+  </si>
+  <si>
+    <t>Region</t>
+  </si>
+  <si>
+    <t>South Pacific</t>
+  </si>
+  <si>
+    <t>APAC</t>
   </si>
 </sst>
 </file>
@@ -558,7 +567,7 @@
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J4" sqref="A1:J4"/>
+      <selection activeCell="A6" sqref="A6:E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -859,9 +868,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9489E7BA-1628-4408-A284-66848C1ED495}">
   <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D9" sqref="D9"/>
+      <selection pane="bottomLeft" activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1361,11 +1370,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0495ED7-CB58-49F3-9615-ED578CE24D86}">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G3" sqref="G3"/>
+      <selection pane="bottomLeft" activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1430,9 +1439,11 @@
       <c r="E2" t="s">
         <v>38</v>
       </c>
-      <c r="F2" s="2"/>
+      <c r="F2" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="G2" s="2" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="I2" t="s">
         <v>34</v>
@@ -1454,18 +1465,78 @@
       <c r="E3" t="s">
         <v>38</v>
       </c>
-      <c r="F3" s="2"/>
+      <c r="F3" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="G3" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="I3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="I3" t="s">
-        <v>34</v>
+      <c r="G4" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="I4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1" xr:uid="{496E8D72-0232-4903-AC23-C02DA08108A7}"/>
-    <hyperlink ref="G3" r:id="rId2" xr:uid="{8DF27D09-716D-4D4B-BAB9-9EB26B5534EB}"/>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{496E8D72-0232-4903-AC23-C02DA08108A7}"/>
+    <hyperlink ref="F3" r:id="rId2" xr:uid="{8DF27D09-716D-4D4B-BAB9-9EB26B5534EB}"/>
+    <hyperlink ref="F4" r:id="rId3" xr:uid="{BCAD9E02-EA55-4732-B4A9-1DF186805468}"/>
+    <hyperlink ref="G2" r:id="rId4" xr:uid="{81A734D9-C7FB-4C01-8DF8-6452DCCAAA9F}"/>
+    <hyperlink ref="G3" r:id="rId5" xr:uid="{FA499D61-9975-4912-A1EF-9725B0A5945B}"/>
+    <hyperlink ref="G4" r:id="rId6" xr:uid="{DF08651E-81CD-4A9D-AC08-2326C06306FE}"/>
+    <hyperlink ref="F5" r:id="rId7" xr:uid="{24F30F30-6258-4C17-95AF-E9CDB50DDDA8}"/>
+    <hyperlink ref="G5" r:id="rId8" xr:uid="{D7CFE1E3-DADF-499F-8BEA-439EE9602BAA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
implemented insight level Upper Extremities
</commit_message>
<xml_diff>
--- a/map.xlsx
+++ b/map.xlsx
@@ -1,22 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stryker-my.sharepoint.com/personal/swastik_mishra_stryker_com/Documents/python/autoinsights/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="76" documentId="13_ncr:1_{FEDAD199-E267-4A23-A1C7-5876348D1EB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D0C30C8F-6888-4BE0-9356-D727DCBB1F7A}"/>
+  <xr:revisionPtr revIDLastSave="166" documentId="13_ncr:1_{FEDAD199-E267-4A23-A1C7-5876348D1EB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4CB44AB2-9CCE-442C-9E22-61E7D60F3F71}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet5" sheetId="5" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="14" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="15" r:id="rId4"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet5!$A$1:$J$1</definedName>
+  </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -38,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="43">
   <si>
     <t>Location Hierarchy</t>
   </si>
@@ -157,57 +161,6 @@
     <t>Orthopedics</t>
   </si>
   <si>
-    <t>matthew.wisdom@stryker.com</t>
-  </si>
-  <si>
-    <t>ORTHOLOC 3DI ANKLE FX</t>
-  </si>
-  <si>
-    <t>ORTHOLOC 3DI ANKLE FX LP</t>
-  </si>
-  <si>
-    <t>ORTHOLOC 3DI FLATFOOT</t>
-  </si>
-  <si>
-    <t>ORTHOLOC 3DI HALLUX</t>
-  </si>
-  <si>
-    <t>ORTHOLOC 3DI MIDFOOT</t>
-  </si>
-  <si>
-    <t>ORTHOLOC 3DI OTHER</t>
-  </si>
-  <si>
-    <t>ORTHOLOC 3DI SMALL BONE</t>
-  </si>
-  <si>
-    <t>ORTHOLOC CALC FX</t>
-  </si>
-  <si>
-    <t>SMALL BONES OTHER</t>
-  </si>
-  <si>
-    <t>SYNDESMOSIS</t>
-  </si>
-  <si>
-    <t>VARIAX FOOT PLATES</t>
-  </si>
-  <si>
-    <t>BIOFOAM</t>
-  </si>
-  <si>
-    <t>CITRELOCK</t>
-  </si>
-  <si>
-    <t>ENDOTRAC</t>
-  </si>
-  <si>
-    <t>FUTURA CSI</t>
-  </si>
-  <si>
-    <t>SONICFUSION</t>
-  </si>
-  <si>
     <t>Region</t>
   </si>
   <si>
@@ -215,6 +168,9 @@
   </si>
   <si>
     <t>APAC</t>
+  </si>
+  <si>
+    <t>Upper Extremities</t>
   </si>
 </sst>
 </file>
@@ -274,7 +230,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -283,6 +239,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -567,7 +526,7 @@
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:E6"/>
+      <selection activeCell="J2" sqref="A2:J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -866,18 +825,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9489E7BA-1628-4408-A284-66848C1ED495}">
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F17" sqref="F17"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="27.6640625" customWidth="1"/>
+    <col min="2" max="2" width="17.21875" customWidth="1"/>
+    <col min="3" max="3" width="12.5546875" customWidth="1"/>
     <col min="4" max="4" width="34.88671875" customWidth="1"/>
-    <col min="6" max="6" width="24.33203125" customWidth="1"/>
+    <col min="5" max="5" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="51.44140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="21.44140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -914,455 +875,98 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="A2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D2" t="s">
-        <v>40</v>
-      </c>
-      <c r="E2" t="s">
-        <v>38</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>36</v>
+        <v>12</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="I2" t="s">
-        <v>34</v>
+        <v>19</v>
+      </c>
+      <c r="H2" s="3">
+        <v>1</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D3" t="s">
-        <v>41</v>
-      </c>
-      <c r="E3" t="s">
-        <v>38</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="I3" t="s">
-        <v>34</v>
-      </c>
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" t="s">
-        <v>42</v>
-      </c>
-      <c r="E4" t="s">
-        <v>38</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="I4" t="s">
-        <v>34</v>
-      </c>
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D5" t="s">
-        <v>43</v>
-      </c>
-      <c r="E5" t="s">
-        <v>38</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="I5" t="s">
-        <v>34</v>
-      </c>
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D6" t="s">
-        <v>44</v>
-      </c>
-      <c r="E6" t="s">
-        <v>38</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="I6" t="s">
-        <v>34</v>
-      </c>
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D7" t="s">
-        <v>45</v>
-      </c>
-      <c r="E7" t="s">
-        <v>38</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="I7" t="s">
-        <v>34</v>
-      </c>
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D8" t="s">
-        <v>46</v>
-      </c>
-      <c r="E8" t="s">
-        <v>38</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="I8" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9" t="s">
-        <v>47</v>
-      </c>
-      <c r="E9" t="s">
-        <v>38</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="I9" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D10" t="s">
-        <v>48</v>
-      </c>
-      <c r="E10" t="s">
-        <v>38</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="I10" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D11" t="s">
-        <v>49</v>
-      </c>
-      <c r="E11" t="s">
-        <v>38</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="I11" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D12" t="s">
-        <v>50</v>
-      </c>
-      <c r="E12" t="s">
-        <v>38</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="I12" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>10</v>
-      </c>
-      <c r="B13" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D13" t="s">
-        <v>51</v>
-      </c>
-      <c r="E13" t="s">
-        <v>38</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="I13" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>10</v>
-      </c>
-      <c r="B14" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D14" t="s">
-        <v>52</v>
-      </c>
-      <c r="E14" t="s">
-        <v>38</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="I14" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>10</v>
-      </c>
-      <c r="B15" t="s">
-        <v>11</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D15" t="s">
-        <v>53</v>
-      </c>
-      <c r="E15" t="s">
-        <v>38</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="I15" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>10</v>
-      </c>
-      <c r="B16" t="s">
-        <v>11</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D16" t="s">
-        <v>54</v>
-      </c>
-      <c r="E16" t="s">
-        <v>38</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="I16" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>10</v>
-      </c>
-      <c r="B17" t="s">
-        <v>11</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D17" t="s">
-        <v>55</v>
-      </c>
-      <c r="E17" t="s">
-        <v>38</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="I17" t="s">
-        <v>34</v>
-      </c>
+      <c r="E8" s="3"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:J1" xr:uid="{9489E7BA-1628-4408-A284-66848C1ED495}"/>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" xr:uid="{2C74C14B-75EE-43E1-97BE-F3A19C38A914}"/>
-    <hyperlink ref="F3" r:id="rId2" xr:uid="{45ECD210-34BC-48DF-A45D-9081BC64F9EF}"/>
-    <hyperlink ref="F4" r:id="rId3" xr:uid="{86F80915-BB65-4141-9AED-09CA9F371A53}"/>
-    <hyperlink ref="F5" r:id="rId4" xr:uid="{95E970D6-B685-47DB-A3D0-C0B4A95A6614}"/>
-    <hyperlink ref="F6" r:id="rId5" xr:uid="{CAB933C1-8979-47E3-8286-C0608201A454}"/>
-    <hyperlink ref="F7" r:id="rId6" xr:uid="{ECAE0C78-DD46-4152-A58C-24A4F34FD6DB}"/>
-    <hyperlink ref="F8" r:id="rId7" xr:uid="{637ABCE2-2D68-43D9-B871-035BD322D23D}"/>
-    <hyperlink ref="F9" r:id="rId8" xr:uid="{B13DE0D8-CF61-4A9D-9CF5-DD1E52B8236C}"/>
-    <hyperlink ref="F10" r:id="rId9" xr:uid="{FADC4090-4927-44DA-B294-1CC3363DACAA}"/>
-    <hyperlink ref="F11" r:id="rId10" xr:uid="{841683A9-50E5-475C-9204-9BF2E260FE48}"/>
-    <hyperlink ref="F12" r:id="rId11" xr:uid="{A9020940-FD59-4015-806F-5E30953F60C4}"/>
-    <hyperlink ref="F13" r:id="rId12" xr:uid="{9F4828BE-B74A-44EF-8CC2-4E0F522682D0}"/>
-    <hyperlink ref="F14" r:id="rId13" xr:uid="{AB65FF17-B734-4EC1-B3DE-9257DFB1C5BD}"/>
-    <hyperlink ref="F15" r:id="rId14" xr:uid="{E0719288-BD2B-4B1A-AEF4-12AE3741CB0D}"/>
-    <hyperlink ref="F16" r:id="rId15" xr:uid="{6F4C8986-442A-4B66-AA2D-3302F5490ED7}"/>
-    <hyperlink ref="F17" r:id="rId16" xr:uid="{0A6ACF1C-0F25-4965-A383-76D6D340CB07}"/>
-    <hyperlink ref="G2" r:id="rId17" xr:uid="{9207E56D-79FE-458A-BE25-002E123DA75C}"/>
-    <hyperlink ref="G3" r:id="rId18" xr:uid="{A663B67D-24F3-4DA3-9F89-624949483297}"/>
-    <hyperlink ref="G4" r:id="rId19" xr:uid="{707ACA9C-E2EC-45DE-BE3F-5C4F07B2ABD5}"/>
-    <hyperlink ref="G5" r:id="rId20" xr:uid="{243F1F9A-77B0-4CF9-925D-00F64413E03D}"/>
-    <hyperlink ref="G6" r:id="rId21" xr:uid="{9EE9B8BC-AE5F-4854-BDBE-63F9B612405D}"/>
-    <hyperlink ref="G7" r:id="rId22" xr:uid="{7928859D-F8B4-40CF-B461-35AC495CA2D9}"/>
-    <hyperlink ref="G8" r:id="rId23" xr:uid="{DE86209E-C89E-402F-82CB-1B124473F89C}"/>
-    <hyperlink ref="G9" r:id="rId24" xr:uid="{1579F8F0-24F9-4370-9024-0E020683CBF7}"/>
-    <hyperlink ref="G10" r:id="rId25" xr:uid="{F1914FA4-AA08-423D-8522-872149AA91B3}"/>
-    <hyperlink ref="G11" r:id="rId26" xr:uid="{5F76ED9F-5345-4929-9455-D2B492417D29}"/>
-    <hyperlink ref="G12" r:id="rId27" xr:uid="{AD20E9D5-A7A6-447C-8ACB-57066C506399}"/>
-    <hyperlink ref="G13" r:id="rId28" xr:uid="{0CD1E82E-0165-4962-B19B-36127F920B7F}"/>
-    <hyperlink ref="G14" r:id="rId29" xr:uid="{2262EBA7-9A02-4BD0-9BF8-760E57F35B80}"/>
-    <hyperlink ref="G15" r:id="rId30" xr:uid="{F072F568-E996-418E-9C1F-35E29C26A245}"/>
-    <hyperlink ref="G16" r:id="rId31" xr:uid="{0AB53251-F33D-4BD1-991C-DAF45D4202A3}"/>
-    <hyperlink ref="G17" r:id="rId32" xr:uid="{68668252-932F-47A6-AEC2-14B27D56AD4E}"/>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{06FFEA6D-0F78-4B22-AB12-5D2F7EC44C34}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1370,11 +974,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0495ED7-CB58-49F3-9615-ED578CE24D86}">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G2" sqref="G2"/>
+      <selection pane="bottomLeft" activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1477,10 +1081,10 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>56</v>
+        <v>39</v>
       </c>
       <c r="B4" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
       <c r="C4" t="s">
         <v>29</v>
@@ -1495,7 +1099,7 @@
         <v>36</v>
       </c>
       <c r="I4" t="s">
-        <v>58</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
@@ -1526,6 +1130,41 @@
       <c r="I5" t="s">
         <v>17</v>
       </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E6" s="3"/>
+      <c r="F6" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="I6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1537,6 +1176,179 @@
     <hyperlink ref="G4" r:id="rId6" xr:uid="{DF08651E-81CD-4A9D-AC08-2326C06306FE}"/>
     <hyperlink ref="F5" r:id="rId7" xr:uid="{24F30F30-6258-4C17-95AF-E9CDB50DDDA8}"/>
     <hyperlink ref="G5" r:id="rId8" xr:uid="{D7CFE1E3-DADF-499F-8BEA-439EE9602BAA}"/>
+    <hyperlink ref="F6" r:id="rId9" xr:uid="{5B42D959-705A-4D8C-91CF-F55812315587}"/>
+    <hyperlink ref="G6" r:id="rId10" xr:uid="{38FA5EB3-FFBD-4C2D-A431-64E7E7145CCE}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26B38178-1510-4FF6-8CFA-65F0FC413A31}">
+  <dimension ref="A1:J7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G5" sqref="G5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17.109375" customWidth="1"/>
+    <col min="2" max="2" width="16.5546875" customWidth="1"/>
+    <col min="3" max="3" width="18.21875" customWidth="1"/>
+    <col min="4" max="4" width="24.77734375" customWidth="1"/>
+    <col min="5" max="5" width="21.5546875" customWidth="1"/>
+    <col min="6" max="6" width="18.44140625" customWidth="1"/>
+    <col min="7" max="7" width="48.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E2" s="3"/>
+      <c r="G2" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="I2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="I3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" t="s">
+        <v>34</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="I4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E7" s="3"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{16C82F41-17EE-4F60-8CE2-06ABD6BAA86E}"/>
+    <hyperlink ref="G3" r:id="rId2" xr:uid="{EA0F22CE-93B5-4F9F-ADAF-CBCCBB23C033}"/>
+    <hyperlink ref="G4" r:id="rId3" xr:uid="{C9C0A696-FD43-4EB1-BEBA-2EA3E40D8670}"/>
+    <hyperlink ref="G5" r:id="rId4" xr:uid="{712CDCE6-0D8A-4783-8F0F-F01D31AE423F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
dynamic start year for yoy calculation
</commit_message>
<xml_diff>
--- a/map.xlsx
+++ b/map.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stryker-my.sharepoint.com/personal/swastik_mishra_stryker_com/Documents/python/autoinsights/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="166" documentId="13_ncr:1_{FEDAD199-E267-4A23-A1C7-5876348D1EB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4CB44AB2-9CCE-442C-9E22-61E7D60F3F71}"/>
+  <xr:revisionPtr revIDLastSave="209" documentId="13_ncr:1_{FEDAD199-E267-4A23-A1C7-5876348D1EB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4D47C35B-DB3B-4B84-9BC8-09108B45AA06}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,6 +17,7 @@
     <sheet name="Sheet5" sheetId="5" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="14" r:id="rId3"/>
     <sheet name="Sheet3" sheetId="15" r:id="rId4"/>
+    <sheet name="Sheet4" sheetId="16" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet5!$A$1:$J$1</definedName>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="49">
   <si>
     <t>Location Hierarchy</t>
   </si>
@@ -171,13 +172,31 @@
   </si>
   <si>
     <t>Upper Extremities</t>
+  </si>
+  <si>
+    <t>Endoscopy</t>
+  </si>
+  <si>
+    <t>Sports Medicine</t>
+  </si>
+  <si>
+    <t>Sustainability Solutions</t>
+  </si>
+  <si>
+    <t>carly.keane@stryker.com</t>
+  </si>
+  <si>
+    <t>cole.smith@stryker.com</t>
+  </si>
+  <si>
+    <t>Phuong.Nguyen1@stryker.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -208,6 +227,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -230,7 +255,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -242,6 +267,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -526,7 +552,7 @@
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J2" sqref="A2:J2"/>
+      <selection activeCell="A2" sqref="A2:J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -976,9 +1002,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0495ED7-CB58-49F3-9615-ED578CE24D86}">
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G6" sqref="G6"/>
+      <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1156,15 +1182,31 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
+      <c r="A7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>31</v>
+      </c>
       <c r="G7" s="2"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
+      <c r="H7" s="3">
+        <v>1</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>17</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1178,6 +1220,7 @@
     <hyperlink ref="G5" r:id="rId8" xr:uid="{D7CFE1E3-DADF-499F-8BEA-439EE9602BAA}"/>
     <hyperlink ref="F6" r:id="rId9" xr:uid="{5B42D959-705A-4D8C-91CF-F55812315587}"/>
     <hyperlink ref="G6" r:id="rId10" xr:uid="{38FA5EB3-FFBD-4C2D-A431-64E7E7145CCE}"/>
+    <hyperlink ref="F7" r:id="rId11" xr:uid="{A27DEEFC-8D55-4024-876B-24129EDB89E4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1189,7 +1232,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G5" sqref="G5"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1244,17 +1287,172 @@
         <v>11</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" s="3"/>
+      <c r="F2" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="I2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
         <v>12</v>
       </c>
+      <c r="D3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="I3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="I4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G4" r:id="rId1" display="mailto:Phuong.Nguyen1@stryker.com" xr:uid="{4D710827-C90E-45DF-9A9E-B7F7390555AC}"/>
+    <hyperlink ref="F4" r:id="rId2" xr:uid="{D17FD14C-D3C7-49E5-9E6F-50FE1CCFF49C}"/>
+    <hyperlink ref="F3" r:id="rId3" xr:uid="{CFE103C4-EDEB-4C2E-A32F-62B754ABDC2A}"/>
+    <hyperlink ref="F2" r:id="rId4" xr:uid="{248EDB49-7024-47DB-B75A-25FB73DCB3C0}"/>
+    <hyperlink ref="G3" r:id="rId5" display="mailto:cole.smith@stryker.com" xr:uid="{9DD2765F-481B-4E02-9E77-00CA9F06041B}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13547861-BBDC-4D47-8467-641933C873F6}">
+  <dimension ref="A1:J5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>29</v>
+      </c>
       <c r="D2" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E2" s="3"/>
       <c r="G2" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="I2" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -1273,8 +1471,9 @@
       <c r="E3" t="s">
         <v>38</v>
       </c>
+      <c r="F3" s="2"/>
       <c r="G3" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="I3" t="s">
         <v>34</v>
@@ -1293,8 +1492,9 @@
       <c r="D4" t="s">
         <v>34</v>
       </c>
+      <c r="F4" s="2"/>
       <c r="G4" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="I4" t="s">
         <v>41</v>
@@ -1310,45 +1510,27 @@
       <c r="C5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D5" t="s">
-        <v>23</v>
+      <c r="D5" s="3" t="s">
+        <v>13</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>14</v>
       </c>
+      <c r="F5" s="2"/>
       <c r="G5" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="H5">
-        <v>1</v>
-      </c>
-      <c r="I5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H5" s="3">
+        <v>1</v>
+      </c>
+      <c r="I5" s="3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="E7" s="3"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1" xr:uid="{16C82F41-17EE-4F60-8CE2-06ABD6BAA86E}"/>
-    <hyperlink ref="G3" r:id="rId2" xr:uid="{EA0F22CE-93B5-4F9F-ADAF-CBCCBB23C033}"/>
-    <hyperlink ref="G4" r:id="rId3" xr:uid="{C9C0A696-FD43-4EB1-BEBA-2EA3E40D8670}"/>
-    <hyperlink ref="G5" r:id="rId4" xr:uid="{712CDCE6-0D8A-4783-8F0F-F01D31AE423F}"/>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{E6A8FA41-3353-44B5-BFCE-E9A0B567D007}"/>
+    <hyperlink ref="G3:G5" r:id="rId2" display="swastik.mishra@stryker.com" xr:uid="{A0890DBE-3CC9-44BD-B70C-DDBD11DD7F6F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>